<commit_message>
Modificaciones en enpoints de incidencis
</commit_message>
<xml_diff>
--- a/reconexiones.xlsx
+++ b/reconexiones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JEFFERSON\Downloads\Backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90648A73-ABFC-4C87-BA69-E302E3F6A79B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47362589-C625-47A9-ACA0-B78279DA3687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FEC1CEFE-428D-4480-B2C8-DD51C6A5E488}"/>
   </bookViews>
@@ -141,12 +141,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -161,7 +167,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -169,10 +175,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -491,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1F63DEF-8F3C-46F7-9343-804CE782A2A1}">
   <dimension ref="A1:G550"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -521,13 +530,13 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>11160</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>45876</v>
       </c>
       <c r="E2" s="1"/>
@@ -536,13 +545,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>10527</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>45876</v>
       </c>
       <c r="E3" s="1"/>
@@ -551,13 +560,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>10831</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>45876</v>
       </c>
       <c r="E4" s="1"/>
@@ -566,13 +575,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>50260</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>45876</v>
       </c>
       <c r="E5" s="1"/>
@@ -581,13 +590,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>1180</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>1408013656</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>45882</v>
       </c>
       <c r="E6" s="1"/>
@@ -596,13 +605,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>20062</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>45890</v>
       </c>
       <c r="E7" s="1"/>
@@ -611,13 +620,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>120370</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>45891</v>
       </c>
       <c r="E8" s="1"/>
@@ -626,13 +635,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>67</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>45889</v>
       </c>
       <c r="E9" s="1"/>
@@ -641,13 +650,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>3482</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>45885</v>
       </c>
       <c r="E10" s="1"/>
@@ -656,13 +665,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>19695</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <v>45885</v>
       </c>
       <c r="E11" s="1"/>
@@ -671,13 +680,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>40383</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <v>45885</v>
       </c>
       <c r="E12" s="1"/>
@@ -686,13 +695,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
-      <c r="B13" s="3">
+      <c r="B13" s="2">
         <v>1243</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>17005273</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="3">
         <v>45885</v>
       </c>
       <c r="E13" s="1"/>
@@ -701,13 +710,13 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="2"/>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <v>1259</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <v>17005583</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="3">
         <v>45885</v>
       </c>
       <c r="E14" s="1"/>
@@ -716,13 +725,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="2"/>
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <v>1029</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <v>17005867</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="3">
         <v>45885</v>
       </c>
       <c r="E15" s="1"/>
@@ -731,13 +740,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
-      <c r="B16" s="3">
+      <c r="B16" s="2">
         <v>3237</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="3">
         <v>45885</v>
       </c>
       <c r="E16" s="1"/>
@@ -746,13 +755,13 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
-      <c r="B17" s="3">
+      <c r="B17" s="2">
         <v>3900</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="2">
         <v>2215004304</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="3">
         <v>45885</v>
       </c>
       <c r="E17" s="1"/>
@@ -761,13 +770,13 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="2"/>
-      <c r="B18" s="3">
+      <c r="B18" s="2">
         <v>3659</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="3">
         <v>45887</v>
       </c>
       <c r="E18" s="1"/>
@@ -775,13 +784,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="2"/>
-      <c r="B19" s="3">
+      <c r="B19" s="2">
         <v>20509</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="2">
         <v>2381361930</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D19" s="3">
         <v>45887</v>
       </c>
       <c r="E19" s="1"/>
@@ -789,13 +798,13 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="2"/>
-      <c r="B20" s="3">
+      <c r="B20" s="4">
         <v>1499</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="5">
         <v>45891</v>
       </c>
       <c r="E20" s="1"/>
@@ -803,13 +812,13 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="2"/>
-      <c r="B21" s="3">
+      <c r="B21" s="2">
         <v>3977</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="2">
         <v>2215003920</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="3">
         <v>45884</v>
       </c>
       <c r="E21" s="1"/>
@@ -817,13 +826,13 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="2"/>
-      <c r="B22" s="3">
+      <c r="B22" s="2">
         <v>1385</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="3">
         <v>45897</v>
       </c>
       <c r="E22" s="1"/>
@@ -831,13 +840,13 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
-      <c r="B23" s="3">
+      <c r="B23" s="2">
         <v>3253</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23" s="3">
         <v>45897</v>
       </c>
       <c r="E23" s="1"/>
@@ -845,13 +854,13 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="2"/>
-      <c r="B24" s="3">
+      <c r="B24" s="2">
         <v>10612</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D24" s="3">
         <v>45895</v>
       </c>
       <c r="E24" s="1"/>
@@ -859,13 +868,13 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="2"/>
-      <c r="B25" s="3">
+      <c r="B25" s="2">
         <v>50206</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D25" s="3">
         <v>45895</v>
       </c>
       <c r="E25" s="1"/>
@@ -873,13 +882,13 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="2"/>
-      <c r="B26" s="3">
+      <c r="B26" s="2">
         <v>4319</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="2">
         <v>2215004150</v>
       </c>
-      <c r="D26" s="4">
+      <c r="D26" s="3">
         <v>45895</v>
       </c>
       <c r="E26" s="1"/>
@@ -887,13 +896,13 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
-      <c r="B27" s="3">
+      <c r="B27" s="2">
         <v>547</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D27" s="4">
+      <c r="D27" s="3">
         <v>45895</v>
       </c>
       <c r="E27" s="1"/>
@@ -901,13 +910,13 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="2"/>
-      <c r="B28" s="3">
+      <c r="B28" s="2">
         <v>50209</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D28" s="3">
         <v>45896</v>
       </c>
       <c r="E28" s="1"/>
@@ -915,13 +924,13 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="2"/>
-      <c r="B29" s="3">
+      <c r="B29" s="2">
         <v>50205</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D29" s="4">
+      <c r="D29" s="3">
         <v>45896</v>
       </c>
       <c r="E29" s="1"/>
@@ -929,13 +938,13 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="2"/>
-      <c r="B30" s="3">
+      <c r="B30" s="2">
         <v>2725</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D30" s="3">
         <v>45894</v>
       </c>
       <c r="E30" s="1"/>
@@ -943,13 +952,13 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="2"/>
-      <c r="B31" s="3">
+      <c r="B31" s="2">
         <v>815</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D31" s="4">
+      <c r="D31" s="3">
         <v>45890</v>
       </c>
       <c r="E31" s="1"/>
@@ -957,13 +966,13 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="2"/>
-      <c r="B32" s="3">
+      <c r="B32" s="2">
         <v>110024</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D32" s="4">
+      <c r="D32" s="3">
         <v>45890</v>
       </c>
       <c r="E32" s="1"/>
@@ -971,13 +980,13 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="2"/>
-      <c r="B33" s="3">
+      <c r="B33" s="2">
         <v>3610</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D33" s="4">
+      <c r="D33" s="3">
         <v>45890</v>
       </c>
       <c r="E33" s="1"/>
@@ -985,13 +994,13 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="2"/>
-      <c r="B34" s="3">
+      <c r="B34" s="2">
         <v>3466</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D34" s="4">
+      <c r="D34" s="3">
         <v>45890</v>
       </c>
       <c r="E34" s="1"/>
@@ -999,13 +1008,13 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="2"/>
-      <c r="B35" s="3">
+      <c r="B35" s="2">
         <v>30407</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D35" s="4">
+      <c r="D35" s="3">
         <v>45890</v>
       </c>
       <c r="E35" s="1"/>
@@ -1013,13 +1022,13 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="2"/>
-      <c r="B36" s="3">
+      <c r="B36" s="2">
         <v>50296</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D36" s="4">
+      <c r="D36" s="3">
         <v>45890</v>
       </c>
       <c r="E36" s="1"/>
@@ -1027,13 +1036,13 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="2"/>
-      <c r="B37" s="3">
+      <c r="B37" s="2">
         <v>297</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D37" s="4">
+      <c r="D37" s="3">
         <v>45889</v>
       </c>
       <c r="E37" s="1"/>
@@ -1041,13 +1050,13 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="2"/>
-      <c r="B38" s="3">
+      <c r="B38" s="2">
         <v>892</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C38" s="2">
         <v>17006160</v>
       </c>
-      <c r="D38" s="4">
+      <c r="D38" s="3">
         <v>45889</v>
       </c>
       <c r="E38" s="1"/>

</xml_diff>